<commit_message>
configured mission variables as OpenMDAO vars
</commit_message>
<xml_diff>
--- a/examples/mtow_estimation/estimate_mtow.xlsx
+++ b/examples/mtow_estimation/estimate_mtow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/examples/mtow_estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A8BBFD-BFAF-0D48-B409-0944FA098126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DC1EE-B99A-E047-AF77-5211844AF0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" activeTab="5" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
+    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
   </bookViews>
   <sheets>
     <sheet name="multirotor_fidelity0" sheetId="13" r:id="rId1"/>
@@ -1293,18 +1293,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1313,13 +1301,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1331,25 +1340,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -15423,8 +15423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE37D87-B951-4841-B7CA-13CC46090773}">
   <dimension ref="B1:AO56"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15468,11 +15468,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -15483,26 +15483,26 @@
       </c>
     </row>
     <row r="3" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="F3" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="N3" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
       <c r="U3" s="7" t="s">
         <v>44</v>
       </c>
@@ -15901,11 +15901,11 @@
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
       <c r="N7" t="s">
         <v>123</v>
       </c>
@@ -16334,11 +16334,11 @@
       <c r="H11" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="J11" s="57" t="s">
+      <c r="J11" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
       <c r="N11" s="6" t="s">
         <v>118</v>
       </c>
@@ -16423,11 +16423,11 @@
       </c>
     </row>
     <row r="12" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
       <c r="F12" s="42" t="s">
         <v>85</v>
       </c>
@@ -16545,11 +16545,11 @@
       <c r="L13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="57" t="s">
+      <c r="N13" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
       <c r="U13" s="2">
         <v>9</v>
       </c>
@@ -16636,11 +16636,11 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
       <c r="J14" s="12" t="s">
         <v>135</v>
       </c>
@@ -16945,11 +16945,11 @@
       </c>
     </row>
     <row r="17" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
       <c r="F17" s="6" t="s">
         <v>133</v>
       </c>
@@ -16970,11 +16970,11 @@
       <c r="L17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="57" t="s">
+      <c r="N17" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
       <c r="U17" s="2">
         <v>13</v>
       </c>
@@ -17706,16 +17706,16 @@
       </c>
     </row>
     <row r="24" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="F24" s="57" t="s">
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="F24" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
       <c r="J24" s="15" t="s">
         <v>68</v>
       </c>
@@ -18253,11 +18253,11 @@
       </c>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
       <c r="F29" t="s">
         <v>100</v>
       </c>
@@ -18368,11 +18368,11 @@
       <c r="H30" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="J30" s="54" t="s">
+      <c r="J30" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
       <c r="U30" s="2">
         <v>26</v>
       </c>
@@ -18658,11 +18658,11 @@
         <v>0.80011066800000008</v>
       </c>
       <c r="D33"/>
-      <c r="F33" s="57" t="s">
+      <c r="F33" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
       <c r="J33" s="19" t="s">
         <v>81</v>
       </c>
@@ -18847,11 +18847,11 @@
       </c>
     </row>
     <row r="35" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
       <c r="F35" s="44" t="s">
         <v>225</v>
       </c>
@@ -19017,11 +19017,11 @@
       <c r="C38" s="17">
         <v>0.8</v>
       </c>
-      <c r="J38" s="54" t="s">
+      <c r="J38" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
       <c r="AF38" s="2">
         <v>34</v>
       </c>
@@ -19108,11 +19108,11 @@
       </c>
     </row>
     <row r="40" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
       <c r="J40" s="11" t="s">
         <v>55</v>
       </c>
@@ -19407,16 +19407,16 @@
       </c>
     </row>
     <row r="46" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="J46" s="54" t="s">
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="J46" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="K46" s="54"/>
-      <c r="L46" s="54"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
       <c r="N46" s="6" t="s">
         <v>283</v>
       </c>
@@ -19530,11 +19530,11 @@
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B52" s="54" t="s">
+      <c r="B52" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
@@ -19570,6 +19570,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="F33:H33"/>
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
@@ -19582,17 +19593,6 @@
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="N13:P13"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="F33:H33"/>
   </mergeCells>
   <conditionalFormatting sqref="K28">
     <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="FALSE">
@@ -19624,7 +19624,7 @@
   <dimension ref="B1:AS68"/>
   <sheetViews>
     <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19673,11 +19673,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="2:45" x14ac:dyDescent="0.2">
       <c r="Y2" s="16" t="s">
@@ -19688,31 +19688,31 @@
       </c>
     </row>
     <row r="3" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="F3" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="N3" s="58" t="s">
         <v>279</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="R3" s="54" t="s">
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="R3" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
       <c r="Y3" s="7" t="s">
         <v>44</v>
       </c>
@@ -20136,11 +20136,11 @@
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
       <c r="N7" t="s">
         <v>123</v>
       </c>
@@ -20602,11 +20602,11 @@
       <c r="H11" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="J11" s="57" t="s">
+      <c r="J11" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
       <c r="N11" s="6" t="s">
         <v>118</v>
       </c>
@@ -20697,11 +20697,11 @@
       </c>
     </row>
     <row r="12" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
       <c r="F12" t="s">
         <v>281</v>
       </c>
@@ -20826,16 +20826,16 @@
       <c r="L13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="57" t="s">
+      <c r="N13" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="R13" s="57" t="s">
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="R13" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
       <c r="Y13" s="2">
         <v>9</v>
       </c>
@@ -21145,11 +21145,11 @@
       </c>
     </row>
     <row r="16" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="F16" s="57" t="s">
+      <c r="F16" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
       <c r="J16" s="13" t="s">
         <v>56</v>
       </c>
@@ -21237,11 +21237,11 @@
       </c>
     </row>
     <row r="17" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
       <c r="F17" s="9" t="s">
         <v>92</v>
       </c>
@@ -21262,16 +21262,16 @@
       <c r="L17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="57" t="s">
+      <c r="N17" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="R17" s="57" t="s">
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="R17" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="S17" s="59"/>
-      <c r="T17" s="59"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
       <c r="Y17" s="2">
         <v>13</v>
       </c>
@@ -22063,11 +22063,11 @@
       </c>
     </row>
     <row r="24" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
       <c r="F24" s="44" t="s">
         <v>225</v>
       </c>
@@ -22302,11 +22302,11 @@
       <c r="D26" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="57" t="s">
+      <c r="F26" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
       <c r="J26" s="15" t="s">
         <v>70</v>
       </c>
@@ -22640,11 +22640,11 @@
       </c>
     </row>
     <row r="29" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
       <c r="F29" t="s">
         <v>93</v>
       </c>
@@ -22762,11 +22762,11 @@
       <c r="H30" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="54" t="s">
+      <c r="J30" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
       <c r="Y30" s="2">
         <v>26</v>
       </c>
@@ -23246,16 +23246,16 @@
       </c>
     </row>
     <row r="35" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="F35" s="57" t="s">
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="F35" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
       <c r="J35" s="15" t="s">
         <v>73</v>
       </c>
@@ -23464,11 +23464,11 @@
       <c r="C38" s="17">
         <v>0.8</v>
       </c>
-      <c r="J38" s="54" t="s">
+      <c r="J38" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
       <c r="Y38" s="2">
         <v>0</v>
       </c>
@@ -23631,11 +23631,11 @@
       </c>
     </row>
     <row r="40" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
       <c r="J40" s="11" t="s">
         <v>55</v>
       </c>
@@ -24148,16 +24148,16 @@
       </c>
     </row>
     <row r="46" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="J46" s="54" t="s">
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="J46" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="K46" s="54"/>
-      <c r="L46" s="54"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
       <c r="Y46" s="2">
         <v>8</v>
       </c>
@@ -24480,11 +24480,11 @@
       </c>
     </row>
     <row r="52" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B52" s="54" t="s">
+      <c r="B52" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
       <c r="Y52" s="2">
         <v>14</v>
       </c>
@@ -25207,16 +25207,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="J7:L7"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="J46:L46"/>
@@ -25233,6 +25223,16 @@
     <mergeCell ref="J38:L38"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="J11:L11"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <conditionalFormatting sqref="K28">
     <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="FALSE">
@@ -25263,8 +25263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3661B753-A267-5243-ABFD-E2825908B8D2}">
   <dimension ref="B1:CI136"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25342,11 +25342,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="2:87" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -25414,26 +25414,26 @@
       <c r="CI2" s="61"/>
     </row>
     <row r="3" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="F3" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="N3" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
       <c r="U3" s="7" t="s">
         <v>44</v>
       </c>
@@ -25516,29 +25516,29 @@
         <v>8</v>
       </c>
       <c r="AX3"/>
-      <c r="AY3" s="63" t="s">
+      <c r="AY3" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="AZ3" s="63"/>
-      <c r="BA3" s="63"/>
+      <c r="AZ3" s="62"/>
+      <c r="BA3" s="62"/>
       <c r="BB3"/>
-      <c r="BC3" s="63" t="s">
+      <c r="BC3" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="BD3" s="63"/>
-      <c r="BE3" s="63"/>
+      <c r="BD3" s="62"/>
+      <c r="BE3" s="62"/>
       <c r="BF3"/>
-      <c r="BG3" s="63" t="s">
+      <c r="BG3" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="BH3" s="63"/>
-      <c r="BI3" s="63"/>
+      <c r="BH3" s="62"/>
+      <c r="BI3" s="62"/>
       <c r="BJ3" s="2"/>
-      <c r="BK3" s="63" t="s">
+      <c r="BK3" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="BL3" s="63"/>
-      <c r="BM3" s="63"/>
+      <c r="BL3" s="62"/>
+      <c r="BM3" s="62"/>
       <c r="BN3"/>
       <c r="BO3" s="7" t="s">
         <v>44</v>
@@ -26323,11 +26323,11 @@
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
       <c r="N7" t="s">
         <v>123</v>
       </c>
@@ -27273,11 +27273,11 @@
       <c r="H11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="57" t="s">
+      <c r="J11" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
       <c r="N11" s="6" t="s">
         <v>118</v>
       </c>
@@ -27360,7 +27360,7 @@
         <f t="shared" si="20"/>
         <v>70.3125</v>
       </c>
-      <c r="AQ11" s="67" t="s">
+      <c r="AQ11" s="64" t="s">
         <v>181</v>
       </c>
       <c r="AR11" s="3" t="s">
@@ -27480,11 +27480,11 @@
       </c>
     </row>
     <row r="12" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
       <c r="F12" s="6" t="s">
         <v>217</v>
       </c>
@@ -27577,7 +27577,7 @@
         <f t="shared" si="20"/>
         <v>35.15625</v>
       </c>
-      <c r="AQ12" s="67"/>
+      <c r="AQ12" s="64"/>
       <c r="AR12" s="3" t="s">
         <v>219</v>
       </c>
@@ -27594,17 +27594,17 @@
         <v>104</v>
       </c>
       <c r="AX12"/>
-      <c r="AY12" s="63" t="s">
+      <c r="AY12" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="AZ12" s="63"/>
-      <c r="BA12" s="63"/>
+      <c r="AZ12" s="62"/>
+      <c r="BA12" s="62"/>
       <c r="BB12"/>
-      <c r="BC12" s="63" t="s">
+      <c r="BC12" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="BD12" s="63"/>
-      <c r="BE12" s="63"/>
+      <c r="BD12" s="62"/>
+      <c r="BE12" s="62"/>
       <c r="BF12"/>
       <c r="BG12" s="2" t="s">
         <v>187</v>
@@ -27729,11 +27729,11 @@
       <c r="L13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="57" t="s">
+      <c r="N13" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
       <c r="U13" s="2">
         <v>9</v>
       </c>
@@ -27809,7 +27809,7 @@
         <f t="shared" si="20"/>
         <v>17.578125</v>
       </c>
-      <c r="AQ13" s="67"/>
+      <c r="AQ13" s="64"/>
       <c r="AR13" s="3" t="s">
         <v>219</v>
       </c>
@@ -28038,7 +28038,7 @@
         <f t="shared" si="20"/>
         <v>8.7890625</v>
       </c>
-      <c r="AQ14" s="67"/>
+      <c r="AQ14" s="64"/>
       <c r="AR14" s="3" t="s">
         <v>219</v>
       </c>
@@ -28171,11 +28171,11 @@
       <c r="C15" s="17">
         <v>1</v>
       </c>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
       <c r="J15" s="12" t="s">
         <v>136</v>
       </c>
@@ -28268,7 +28268,7 @@
         <f t="shared" si="20"/>
         <v>4.39453125</v>
       </c>
-      <c r="AQ15" s="67"/>
+      <c r="AQ15" s="64"/>
       <c r="AR15" s="3" t="s">
         <v>219</v>
       </c>
@@ -28499,7 +28499,7 @@
         <f t="shared" si="20"/>
         <v>2.197265625</v>
       </c>
-      <c r="AQ16" s="67"/>
+      <c r="AQ16" s="64"/>
       <c r="AR16" s="3" t="s">
         <v>219</v>
       </c>
@@ -28629,11 +28629,11 @@
       </c>
     </row>
     <row r="17" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
       <c r="F17" t="s">
         <v>130</v>
       </c>
@@ -28654,11 +28654,11 @@
       <c r="L17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="57" t="s">
+      <c r="N17" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
       <c r="U17" s="2">
         <v>13</v>
       </c>
@@ -28734,7 +28734,7 @@
         <f t="shared" si="20"/>
         <v>1.0986328125</v>
       </c>
-      <c r="AQ17" s="67"/>
+      <c r="AQ17" s="64"/>
       <c r="AR17" s="3" t="s">
         <v>219</v>
       </c>
@@ -28971,7 +28971,7 @@
         <f t="shared" si="20"/>
         <v>0.54931640625</v>
       </c>
-      <c r="AQ18" s="67"/>
+      <c r="AQ18" s="64"/>
       <c r="AR18" s="3" t="s">
         <v>219</v>
       </c>
@@ -29212,7 +29212,7 @@
         <f t="shared" si="20"/>
         <v>0.274658203125</v>
       </c>
-      <c r="AQ19" s="67" t="s">
+      <c r="AQ19" s="64" t="s">
         <v>195</v>
       </c>
       <c r="AR19" s="3">
@@ -29459,7 +29459,7 @@
         <f t="shared" si="20"/>
         <v>0.1373291015625</v>
       </c>
-      <c r="AQ20" s="67"/>
+      <c r="AQ20" s="64"/>
       <c r="AR20" s="3">
         <f>0.285*($AR$9/2)</f>
         <v>1.1399999999999999</v>
@@ -29676,7 +29676,7 @@
         <f t="shared" si="20"/>
         <v>6.866455078125E-2</v>
       </c>
-      <c r="AQ21" s="67"/>
+      <c r="AQ21" s="64"/>
       <c r="AR21" s="3">
         <f>0.395*($AR$9/2)</f>
         <v>1.58</v>
@@ -29689,17 +29689,17 @@
       <c r="AV21"/>
       <c r="AW21" s="39"/>
       <c r="AX21"/>
-      <c r="AY21" s="63" t="s">
+      <c r="AY21" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="AZ21" s="63"/>
-      <c r="BA21" s="63"/>
+      <c r="AZ21" s="62"/>
+      <c r="BA21" s="62"/>
       <c r="BB21"/>
-      <c r="BC21" s="63" t="s">
+      <c r="BC21" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="BD21" s="63"/>
-      <c r="BE21" s="63"/>
+      <c r="BD21" s="62"/>
+      <c r="BE21" s="62"/>
       <c r="BF21"/>
       <c r="BG21" s="2"/>
       <c r="BH21" s="2"/>
@@ -29793,11 +29793,11 @@
       <c r="D22" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
       <c r="J22" s="14" t="s">
         <v>117</v>
       </c>
@@ -29890,7 +29890,7 @@
         <f t="shared" si="20"/>
         <v>3.4332275390625E-2</v>
       </c>
-      <c r="AQ22" s="67"/>
+      <c r="AQ22" s="64"/>
       <c r="AR22" s="3">
         <f>0.505*($AR$9/2)</f>
         <v>2.02</v>
@@ -29927,17 +29927,17 @@
         <v>8</v>
       </c>
       <c r="BF22"/>
-      <c r="BG22" s="63" t="s">
+      <c r="BG22" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="BH22" s="63"/>
-      <c r="BI22" s="63"/>
+      <c r="BH22" s="62"/>
+      <c r="BI22" s="62"/>
       <c r="BJ22" s="2"/>
-      <c r="BK22" s="63" t="s">
+      <c r="BK22" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="BL22" s="63"/>
-      <c r="BM22" s="63"/>
+      <c r="BL22" s="62"/>
+      <c r="BM22" s="62"/>
       <c r="BN22"/>
       <c r="BO22" s="2">
         <v>18</v>
@@ -30115,7 +30115,7 @@
         <f t="shared" si="20"/>
         <v>1.71661376953125E-2</v>
       </c>
-      <c r="AQ23" s="67"/>
+      <c r="AQ23" s="64"/>
       <c r="AR23" s="3">
         <f>0.615*($AR$9/2)</f>
         <v>2.46</v>
@@ -30124,14 +30124,14 @@
         <v>8</v>
       </c>
       <c r="AT23"/>
-      <c r="AU23" s="70" t="s">
+      <c r="AU23" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="AV23" s="67">
+      <c r="AV23" s="64">
         <f>BH20</f>
         <v>-1.7565500720628791E-9</v>
       </c>
-      <c r="AW23" s="67"/>
+      <c r="AW23" s="64"/>
       <c r="AX23"/>
       <c r="AY23" s="2" t="s">
         <v>158</v>
@@ -30252,11 +30252,11 @@
       </c>
     </row>
     <row r="24" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
       <c r="F24" t="s">
         <v>94</v>
       </c>
@@ -30362,7 +30362,7 @@
         <f t="shared" si="20"/>
         <v>8.58306884765625E-3</v>
       </c>
-      <c r="AQ24" s="67"/>
+      <c r="AQ24" s="64"/>
       <c r="AR24" s="3">
         <f>0.725*($AR$9/2)</f>
         <v>2.9</v>
@@ -30371,12 +30371,12 @@
         <v>8</v>
       </c>
       <c r="AT24"/>
-      <c r="AU24" s="70"/>
-      <c r="AV24" s="67">
+      <c r="AU24" s="63"/>
+      <c r="AV24" s="64">
         <f>BL20</f>
         <v>3.5749579546662247E-9</v>
       </c>
-      <c r="AW24" s="67"/>
+      <c r="AW24" s="64"/>
       <c r="AX24"/>
       <c r="AY24" s="2" t="s">
         <v>163</v>
@@ -30606,7 +30606,7 @@
         <f t="shared" si="20"/>
         <v>4.291534423828125E-3</v>
       </c>
-      <c r="AQ25" s="67"/>
+      <c r="AQ25" s="64"/>
       <c r="AR25" s="3">
         <f>0.835*($AR$9/2)</f>
         <v>3.34</v>
@@ -30615,12 +30615,12 @@
         <v>8</v>
       </c>
       <c r="AT25"/>
-      <c r="AU25" s="70"/>
-      <c r="AV25" s="67">
+      <c r="AU25" s="63"/>
+      <c r="AV25" s="64">
         <f>BH39</f>
         <v>-3.3095017282214201E-9</v>
       </c>
-      <c r="AW25" s="67"/>
+      <c r="AW25" s="64"/>
       <c r="AX25"/>
       <c r="AY25" s="2" t="s">
         <v>167</v>
@@ -30855,7 +30855,7 @@
         <f t="shared" si="20"/>
         <v>2.1457672119140625E-3</v>
       </c>
-      <c r="AQ26" s="67"/>
+      <c r="AQ26" s="64"/>
       <c r="AR26" s="3">
         <f>0.945*($AR$9/2)</f>
         <v>3.78</v>
@@ -30864,12 +30864,12 @@
         <v>8</v>
       </c>
       <c r="AT26"/>
-      <c r="AU26" s="70"/>
-      <c r="AV26" s="67">
+      <c r="AU26" s="63"/>
+      <c r="AV26" s="64">
         <f>BL39</f>
         <v>-3.4190485859175723E-10</v>
       </c>
-      <c r="AW26" s="67"/>
+      <c r="AW26" s="64"/>
       <c r="AX26"/>
       <c r="AY26" s="2" t="s">
         <v>170</v>
@@ -31097,7 +31097,7 @@
         <f t="shared" si="20"/>
         <v>1.0728836059570312E-3</v>
       </c>
-      <c r="AQ27" s="67" t="s">
+      <c r="AQ27" s="64" t="s">
         <v>204</v>
       </c>
       <c r="AR27" s="3">
@@ -31108,12 +31108,12 @@
         <v>8</v>
       </c>
       <c r="AT27"/>
-      <c r="AU27" s="70"/>
-      <c r="AV27" s="67">
+      <c r="AU27" s="63"/>
+      <c r="AV27" s="64">
         <f>BH58</f>
         <v>-5.942139558179349E-10</v>
       </c>
-      <c r="AW27" s="67"/>
+      <c r="AW27" s="64"/>
       <c r="AX27"/>
       <c r="AY27" s="2" t="s">
         <v>174</v>
@@ -31318,7 +31318,7 @@
         <f t="shared" si="20"/>
         <v>5.3644180297851562E-4</v>
       </c>
-      <c r="AQ28" s="67"/>
+      <c r="AQ28" s="64"/>
       <c r="AR28" s="3">
         <f>0.069425*($AR$9/2)</f>
         <v>0.2777</v>
@@ -31327,12 +31327,12 @@
         <v>8</v>
       </c>
       <c r="AT28"/>
-      <c r="AU28" s="70"/>
-      <c r="AV28" s="67">
+      <c r="AU28" s="63"/>
+      <c r="AV28" s="64">
         <f>BL58</f>
         <v>4.158961265654515E-9</v>
       </c>
-      <c r="AW28" s="67"/>
+      <c r="AW28" s="64"/>
       <c r="AX28"/>
       <c r="AY28" s="2" t="s">
         <v>178</v>
@@ -31449,16 +31449,16 @@
       </c>
     </row>
     <row r="29" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="F29" s="57" t="s">
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="F29" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
       <c r="N29" s="6" t="s">
         <v>38</v>
       </c>
@@ -31541,7 +31541,7 @@
         <f t="shared" si="20"/>
         <v>2.6822090148925781E-4</v>
       </c>
-      <c r="AQ29" s="67"/>
+      <c r="AQ29" s="64"/>
       <c r="AR29" s="3">
         <f>0.067375*($AR$9/2)</f>
         <v>0.26950000000000002</v>
@@ -31550,12 +31550,12 @@
         <v>8</v>
       </c>
       <c r="AT29"/>
-      <c r="AU29" s="70"/>
-      <c r="AV29" s="67">
+      <c r="AU29" s="63"/>
+      <c r="AV29" s="64">
         <f>BH77</f>
         <v>1.4573390445804524E-9</v>
       </c>
-      <c r="AW29" s="67"/>
+      <c r="AW29" s="64"/>
       <c r="AX29"/>
       <c r="AY29"/>
       <c r="AZ29"/>
@@ -31674,11 +31674,11 @@
       <c r="H30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J30" s="54" t="s">
+      <c r="J30" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
       <c r="U30" s="2">
         <v>26</v>
       </c>
@@ -31754,7 +31754,7 @@
         <f t="shared" si="20"/>
         <v>1.3411045074462891E-4</v>
       </c>
-      <c r="AQ30" s="67"/>
+      <c r="AQ30" s="64"/>
       <c r="AR30" s="3">
         <f>0.065325*($AR$9/2)</f>
         <v>0.26129999999999998</v>
@@ -31766,23 +31766,23 @@
       <c r="AU30" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="AV30" s="67" t="b">
+      <c r="AV30" s="64" t="b">
         <f>IF(AV23&lt;0.00001,IF(AV24&lt;0.00001,IF(AV25&lt;0.00001,IF(AV26&lt;0.00001,IF(AV27&lt;0.00001,IF(AV28&lt;0.00001,IF(AV29&lt;0.00001,TRUE,FALSE),FALSE),FALSE),FALSE),FALSE),FALSE),FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AW30" s="67"/>
+      <c r="AW30" s="64"/>
       <c r="AX30"/>
-      <c r="AY30" s="63" t="s">
+      <c r="AY30" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="AZ30" s="63"/>
-      <c r="BA30" s="63"/>
+      <c r="AZ30" s="62"/>
+      <c r="BA30" s="62"/>
       <c r="BB30"/>
-      <c r="BC30" s="63" t="s">
+      <c r="BC30" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="BD30" s="63"/>
-      <c r="BE30" s="63"/>
+      <c r="BD30" s="62"/>
+      <c r="BE30" s="62"/>
       <c r="BF30"/>
       <c r="BG30" s="2" t="s">
         <v>183</v>
@@ -31979,7 +31979,7 @@
         <f t="shared" si="20"/>
         <v>6.7055225372314453E-5</v>
       </c>
-      <c r="AQ31" s="67"/>
+      <c r="AQ31" s="64"/>
       <c r="AR31" s="3">
         <f>0.063275*($AR$9/2)</f>
         <v>0.25309999999999999</v>
@@ -32201,7 +32201,7 @@
         <f t="shared" si="20"/>
         <v>3.3527612686157227E-5</v>
       </c>
-      <c r="AQ32" s="67"/>
+      <c r="AQ32" s="64"/>
       <c r="AR32" s="3">
         <f>0.061225*($AR$9/2)</f>
         <v>0.24490000000000001</v>
@@ -32422,7 +32422,7 @@
         <f t="shared" si="20"/>
         <v>1.6763806343078613E-5</v>
       </c>
-      <c r="AQ33" s="67"/>
+      <c r="AQ33" s="64"/>
       <c r="AR33" s="3">
         <f>0.059175*($AR$9/2)</f>
         <v>0.23669999999999999</v>
@@ -32635,7 +32635,7 @@
         <f t="shared" si="20"/>
         <v>8.3819031715393066E-6</v>
       </c>
-      <c r="AQ34" s="67"/>
+      <c r="AQ34" s="64"/>
       <c r="AR34" s="3">
         <f>0.057125*($AR$9/2)</f>
         <v>0.22850000000000001</v>
@@ -32763,11 +32763,11 @@
       </c>
     </row>
     <row r="35" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
       <c r="J35" s="15" t="s">
         <v>73</v>
       </c>
@@ -32814,7 +32814,7 @@
         <f t="shared" si="20"/>
         <v>4.1909515857696533E-6</v>
       </c>
-      <c r="AQ35" s="67" t="s">
+      <c r="AQ35" s="64" t="s">
         <v>223</v>
       </c>
       <c r="AR35" s="3">
@@ -32942,7 +32942,7 @@
         <f t="shared" si="20"/>
         <v>2.0954757928848267E-6</v>
       </c>
-      <c r="AQ36" s="67"/>
+      <c r="AQ36" s="64"/>
       <c r="AR36" s="3">
         <v>5.58</v>
       </c>
@@ -33063,7 +33063,7 @@
         <f t="shared" si="20"/>
         <v>1.0477378964424133E-6</v>
       </c>
-      <c r="AQ37" s="67"/>
+      <c r="AQ37" s="64"/>
       <c r="AR37" s="3">
         <v>4.26</v>
       </c>
@@ -33184,11 +33184,11 @@
       <c r="C38" s="17">
         <v>0.8</v>
       </c>
-      <c r="J38" s="54" t="s">
+      <c r="J38" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
       <c r="AF38" s="2">
         <v>34</v>
       </c>
@@ -33225,7 +33225,7 @@
         <f t="shared" si="20"/>
         <v>5.2386894822120667E-7</v>
       </c>
-      <c r="AQ38" s="67"/>
+      <c r="AQ38" s="64"/>
       <c r="AR38" s="3">
         <v>2.94</v>
       </c>
@@ -33354,7 +33354,7 @@
         <f t="shared" si="20"/>
         <v>2.6193447411060333E-7</v>
       </c>
-      <c r="AQ39" s="67"/>
+      <c r="AQ39" s="64"/>
       <c r="AR39" s="3">
         <v>1.62</v>
       </c>
@@ -33473,11 +33473,11 @@
       </c>
     </row>
     <row r="40" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
       <c r="J40" s="11" t="s">
         <v>55</v>
       </c>
@@ -33524,7 +33524,7 @@
         <f t="shared" si="20"/>
         <v>1.3096723705530167E-7</v>
       </c>
-      <c r="AQ40" s="67"/>
+      <c r="AQ40" s="64"/>
       <c r="AR40" s="3">
         <v>0.3</v>
       </c>
@@ -33682,7 +33682,7 @@
         <f t="shared" si="20"/>
         <v>6.5483618527650833E-8</v>
       </c>
-      <c r="AQ41" s="67"/>
+      <c r="AQ41" s="64"/>
       <c r="AR41" s="3">
         <v>-1.02</v>
       </c>
@@ -33693,10 +33693,10 @@
       <c r="AU41" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="AV41" s="69" t="s">
+      <c r="AV41" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="AW41" s="69"/>
+      <c r="AW41" s="66"/>
       <c r="AX41" s="24"/>
       <c r="AY41" s="24"/>
       <c r="AZ41" s="24"/>
@@ -33706,17 +33706,17 @@
       <c r="BD41" s="24"/>
       <c r="BE41" s="25"/>
       <c r="BF41"/>
-      <c r="BG41" s="63" t="s">
+      <c r="BG41" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="BH41" s="63"/>
-      <c r="BI41" s="63"/>
+      <c r="BH41" s="62"/>
+      <c r="BI41" s="62"/>
       <c r="BJ41" s="2"/>
-      <c r="BK41" s="63" t="s">
+      <c r="BK41" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="BL41" s="63"/>
-      <c r="BM41" s="63"/>
+      <c r="BL41" s="62"/>
+      <c r="BM41" s="62"/>
       <c r="BN41"/>
       <c r="BO41" s="2">
         <v>3</v>
@@ -33848,7 +33848,7 @@
         <f t="shared" si="20"/>
         <v>3.2741809263825417E-8</v>
       </c>
-      <c r="AQ42" s="67"/>
+      <c r="AQ42" s="64"/>
       <c r="AR42" s="3">
         <v>-2.34</v>
       </c>
@@ -33857,22 +33857,22 @@
       </c>
       <c r="AT42"/>
       <c r="AU42" s="27"/>
-      <c r="AV42" s="70" t="s">
+      <c r="AV42" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="AW42" s="70"/>
-      <c r="AX42" s="70"/>
-      <c r="AY42" s="70" t="s">
+      <c r="AW42" s="63"/>
+      <c r="AX42" s="63"/>
+      <c r="AY42" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="AZ42" s="70"/>
-      <c r="BA42" s="70"/>
-      <c r="BB42" s="70"/>
-      <c r="BC42" s="70" t="s">
+      <c r="AZ42" s="63"/>
+      <c r="BA42" s="63"/>
+      <c r="BB42" s="63"/>
+      <c r="BC42" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="BD42" s="70"/>
-      <c r="BE42" s="71"/>
+      <c r="BD42" s="63"/>
+      <c r="BE42" s="65"/>
       <c r="BF42"/>
       <c r="BG42" s="28" t="s">
         <v>154</v>
@@ -34040,10 +34040,10 @@
       <c r="AX43" s="2">
         <v>-9.5</v>
       </c>
-      <c r="AY43" s="70" t="s">
+      <c r="AY43" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="AZ43" s="70"/>
+      <c r="AZ43" s="63"/>
       <c r="BA43" s="2">
         <v>-9.5</v>
       </c>
@@ -34491,11 +34491,11 @@
       </c>
     </row>
     <row r="46" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="AQ46" s="2" t="s">
         <v>31</v>
       </c>
@@ -34621,12 +34621,12 @@
       <c r="D47" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AF47" s="62" t="s">
+      <c r="AF47" s="72" t="s">
         <v>222</v>
       </c>
-      <c r="AG47" s="62"/>
-      <c r="AH47" s="62"/>
-      <c r="AI47" s="62"/>
+      <c r="AG47" s="72"/>
+      <c r="AH47" s="72"/>
+      <c r="AI47" s="72"/>
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
       <c r="AL47" s="2"/>
@@ -34637,10 +34637,10 @@
       <c r="AU47" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="AV47" s="69" t="s">
+      <c r="AV47" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="AW47" s="69"/>
+      <c r="AW47" s="66"/>
       <c r="AX47" s="24"/>
       <c r="AY47" s="24"/>
       <c r="AZ47" s="24"/>
@@ -34784,21 +34784,21 @@
       </c>
       <c r="AT48"/>
       <c r="AU48" s="27"/>
-      <c r="AV48" s="70" t="s">
+      <c r="AV48" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="AW48" s="70"/>
-      <c r="AX48" s="70"/>
-      <c r="AY48" s="70" t="s">
+      <c r="AW48" s="63"/>
+      <c r="AX48" s="63"/>
+      <c r="AY48" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="AZ48" s="70"/>
-      <c r="BA48" s="70"/>
-      <c r="BB48" s="70" t="s">
+      <c r="AZ48" s="63"/>
+      <c r="BA48" s="63"/>
+      <c r="BB48" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="BC48" s="70"/>
-      <c r="BD48" s="70"/>
+      <c r="BC48" s="63"/>
+      <c r="BD48" s="63"/>
       <c r="BE48" s="49"/>
       <c r="BF48"/>
       <c r="BG48" s="2" t="s">
@@ -35095,7 +35095,7 @@
         <v>1450</v>
       </c>
       <c r="AT50"/>
-      <c r="AU50" s="72" t="s">
+      <c r="AU50" s="70" t="s">
         <v>160</v>
       </c>
       <c r="AV50" s="51">
@@ -35257,7 +35257,7 @@
         <v>725</v>
       </c>
       <c r="AT51"/>
-      <c r="AU51" s="72"/>
+      <c r="AU51" s="70"/>
       <c r="AV51" s="27">
         <v>-1.144044407873E-4</v>
       </c>
@@ -35380,11 +35380,11 @@
       </c>
     </row>
     <row r="52" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B52" s="54" t="s">
+      <c r="B52" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
       <c r="AF52" s="2">
         <v>3</v>
       </c>
@@ -35422,22 +35422,22 @@
         <v>362.5</v>
       </c>
       <c r="AT52"/>
-      <c r="AU52" s="72"/>
-      <c r="AV52" s="64">
+      <c r="AU52" s="70"/>
+      <c r="AV52" s="67">
         <v>-2.2751380819795499</v>
       </c>
-      <c r="AW52" s="65"/>
-      <c r="AX52" s="66"/>
-      <c r="AY52" s="64">
+      <c r="AW52" s="68"/>
+      <c r="AX52" s="69"/>
+      <c r="AY52" s="67">
         <v>0.14939144598517301</v>
       </c>
-      <c r="AZ52" s="65"/>
-      <c r="BA52" s="66"/>
-      <c r="BB52" s="67">
+      <c r="AZ52" s="68"/>
+      <c r="BA52" s="69"/>
+      <c r="BB52" s="64">
         <v>3.3811980767955601</v>
       </c>
-      <c r="BC52" s="67"/>
-      <c r="BD52" s="68"/>
+      <c r="BC52" s="64"/>
+      <c r="BD52" s="73"/>
       <c r="BE52" s="27"/>
       <c r="BF52"/>
       <c r="BG52" s="2" t="s">
@@ -35576,7 +35576,7 @@
         <v>181.25</v>
       </c>
       <c r="AT53"/>
-      <c r="AU53" s="72" t="s">
+      <c r="AU53" s="70" t="s">
         <v>164</v>
       </c>
       <c r="AV53" s="51">
@@ -35744,7 +35744,7 @@
         <v>90.625</v>
       </c>
       <c r="AT54"/>
-      <c r="AU54" s="72"/>
+      <c r="AU54" s="70"/>
       <c r="AV54" s="27">
         <v>-3.2678211540000002E-6</v>
       </c>
@@ -35910,22 +35910,22 @@
         <v>45.3125</v>
       </c>
       <c r="AT55"/>
-      <c r="AU55" s="73"/>
-      <c r="AV55" s="64">
+      <c r="AU55" s="71"/>
+      <c r="AV55" s="67">
         <v>-2.92797950805124E-2</v>
       </c>
-      <c r="AW55" s="65"/>
-      <c r="AX55" s="66"/>
-      <c r="AY55" s="65">
+      <c r="AW55" s="68"/>
+      <c r="AX55" s="69"/>
+      <c r="AY55" s="68">
         <v>4.8575804011639703E-2</v>
       </c>
-      <c r="AZ55" s="65"/>
-      <c r="BA55" s="65"/>
-      <c r="BB55" s="64">
+      <c r="AZ55" s="68"/>
+      <c r="BA55" s="68"/>
+      <c r="BB55" s="67">
         <v>7.4720850653456003E-3</v>
       </c>
-      <c r="BC55" s="65"/>
-      <c r="BD55" s="66"/>
+      <c r="BC55" s="68"/>
+      <c r="BD55" s="69"/>
       <c r="BE55"/>
       <c r="BF55"/>
       <c r="BG55" s="2" t="s">
@@ -36634,17 +36634,17 @@
       <c r="BD60"/>
       <c r="BE60"/>
       <c r="BF60"/>
-      <c r="BG60" s="63" t="s">
+      <c r="BG60" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="BH60" s="63"/>
-      <c r="BI60" s="63"/>
+      <c r="BH60" s="62"/>
+      <c r="BI60" s="62"/>
       <c r="BJ60" s="2"/>
-      <c r="BK60" s="63" t="s">
+      <c r="BK60" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="BL60" s="63"/>
-      <c r="BM60" s="63"/>
+      <c r="BL60" s="62"/>
+      <c r="BM60" s="62"/>
       <c r="BN60"/>
       <c r="BO60" s="2">
         <v>22</v>
@@ -38408,7 +38408,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="BU73" s="2">
-        <f t="dataTable" ref="BU73:BU102" dt2D="0" dtr="0" r1="BH42" ca="1"/>
+        <f t="dataTable" ref="BU73:BU102" dt2D="0" dtr="0" r1="BH42"/>
         <v>1.0066183554337029</v>
       </c>
       <c r="BV73" s="2">
@@ -38448,7 +38448,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="CF73" s="2">
-        <f t="dataTable" ref="CF73:CF102" dt2D="0" dtr="0" r1="BL42" ca="1"/>
+        <f t="dataTable" ref="CF73:CF102" dt2D="0" dtr="0" r1="BL42"/>
         <v>1.0074826134077486</v>
       </c>
       <c r="CG73" s="2">
@@ -41894,7 +41894,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="BU107" s="2">
-        <f t="dataTable" ref="BU107:BU136" dt2D="0" dtr="0" r1="BH61" ca="1"/>
+        <f t="dataTable" ref="BU107:BU136" dt2D="0" dtr="0" r1="BH61"/>
         <v>1.0109046148669258</v>
       </c>
       <c r="BV107" s="2">
@@ -41934,7 +41934,7 @@
         <v>1.4152874904422017</v>
       </c>
       <c r="CF107" s="2">
-        <f t="dataTable" ref="CF107:CF136" dt2D="0" dtr="0" r1="BL61" ca="1"/>
+        <f t="dataTable" ref="CF107:CF136" dt2D="0" dtr="0" r1="BL61"/>
         <v>1.0222406911815489</v>
       </c>
       <c r="CG107" s="2">
@@ -44810,62 +44810,20 @@
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="BZ2:CI2"/>
-    <mergeCell ref="AY3:BA3"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BG3:BI3"/>
-    <mergeCell ref="AQ2:AS2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="AY2:BE2"/>
-    <mergeCell ref="BG2:BM2"/>
-    <mergeCell ref="BO2:BX2"/>
-    <mergeCell ref="BK3:BM3"/>
-    <mergeCell ref="BK22:BM22"/>
-    <mergeCell ref="AU23:AU29"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="AV24:AW24"/>
-    <mergeCell ref="AU14:AW14"/>
-    <mergeCell ref="AU22:AW22"/>
-    <mergeCell ref="BG22:BI22"/>
-    <mergeCell ref="AV25:AW25"/>
-    <mergeCell ref="AV26:AW26"/>
-    <mergeCell ref="AV27:AW27"/>
-    <mergeCell ref="AV28:AW28"/>
-    <mergeCell ref="AQ27:AQ34"/>
-    <mergeCell ref="AV29:AW29"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AY30:BA30"/>
-    <mergeCell ref="BC30:BE30"/>
-    <mergeCell ref="AQ7:AS7"/>
-    <mergeCell ref="AU9:AW9"/>
-    <mergeCell ref="AY12:BA12"/>
-    <mergeCell ref="BC12:BE12"/>
-    <mergeCell ref="AY21:BA21"/>
-    <mergeCell ref="BC21:BE21"/>
-    <mergeCell ref="AQ11:AQ18"/>
-    <mergeCell ref="AQ19:AQ26"/>
+    <mergeCell ref="BZ104:CI104"/>
+    <mergeCell ref="AF47:AI47"/>
+    <mergeCell ref="BO104:BX104"/>
+    <mergeCell ref="BG60:BI60"/>
+    <mergeCell ref="BO70:BX70"/>
+    <mergeCell ref="BZ70:CI70"/>
+    <mergeCell ref="AY52:BA52"/>
+    <mergeCell ref="AY55:BA55"/>
+    <mergeCell ref="BB52:BD52"/>
+    <mergeCell ref="BB55:BD55"/>
+    <mergeCell ref="AV47:AW47"/>
+    <mergeCell ref="AV48:AX48"/>
+    <mergeCell ref="AY48:BA48"/>
+    <mergeCell ref="BB48:BD48"/>
     <mergeCell ref="AQ35:AQ42"/>
     <mergeCell ref="AV42:AX42"/>
     <mergeCell ref="BK60:BM60"/>
@@ -44882,20 +44840,62 @@
     <mergeCell ref="AU50:AU52"/>
     <mergeCell ref="AU53:AU55"/>
     <mergeCell ref="AV55:AX55"/>
-    <mergeCell ref="BZ104:CI104"/>
-    <mergeCell ref="AF47:AI47"/>
-    <mergeCell ref="BO104:BX104"/>
-    <mergeCell ref="BG60:BI60"/>
-    <mergeCell ref="BO70:BX70"/>
-    <mergeCell ref="BZ70:CI70"/>
-    <mergeCell ref="AY52:BA52"/>
-    <mergeCell ref="AY55:BA55"/>
-    <mergeCell ref="BB52:BD52"/>
-    <mergeCell ref="BB55:BD55"/>
-    <mergeCell ref="AV47:AW47"/>
-    <mergeCell ref="AV48:AX48"/>
-    <mergeCell ref="AY48:BA48"/>
-    <mergeCell ref="BB48:BD48"/>
+    <mergeCell ref="AQ7:AS7"/>
+    <mergeCell ref="AU9:AW9"/>
+    <mergeCell ref="AY12:BA12"/>
+    <mergeCell ref="BC12:BE12"/>
+    <mergeCell ref="AY21:BA21"/>
+    <mergeCell ref="BC21:BE21"/>
+    <mergeCell ref="AQ11:AQ18"/>
+    <mergeCell ref="AQ19:AQ26"/>
+    <mergeCell ref="AQ27:AQ34"/>
+    <mergeCell ref="AV29:AW29"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AY30:BA30"/>
+    <mergeCell ref="BC30:BE30"/>
+    <mergeCell ref="BK22:BM22"/>
+    <mergeCell ref="AU23:AU29"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="AV24:AW24"/>
+    <mergeCell ref="AU14:AW14"/>
+    <mergeCell ref="AU22:AW22"/>
+    <mergeCell ref="BG22:BI22"/>
+    <mergeCell ref="AV25:AW25"/>
+    <mergeCell ref="AV26:AW26"/>
+    <mergeCell ref="AV27:AW27"/>
+    <mergeCell ref="AV28:AW28"/>
+    <mergeCell ref="BZ2:CI2"/>
+    <mergeCell ref="AY3:BA3"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BG3:BI3"/>
+    <mergeCell ref="AQ2:AS2"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="AY2:BE2"/>
+    <mergeCell ref="BG2:BM2"/>
+    <mergeCell ref="BO2:BX2"/>
+    <mergeCell ref="BK3:BM3"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="G12">
     <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="FALSE">
@@ -44947,7 +44947,7 @@
   <dimension ref="B1:AO81"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44988,11 +44988,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -45003,26 +45003,26 @@
       </c>
     </row>
     <row r="3" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="F3" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="N3" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
       <c r="U3" s="7" t="s">
         <v>44</v>
       </c>
@@ -45644,11 +45644,11 @@
       <c r="H9" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
       <c r="N9" s="6" t="s">
         <v>122</v>
       </c>
@@ -45962,11 +45962,11 @@
       <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
       <c r="N12" s="6" t="s">
         <v>235</v>
       </c>
@@ -46263,11 +46263,11 @@
       </c>
     </row>
     <row r="15" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
       <c r="F15" s="6" t="s">
         <v>240</v>
       </c>
@@ -46617,11 +46617,11 @@
       <c r="L18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N18" s="57" t="s">
+      <c r="N18" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
       <c r="U18" s="2">
         <v>14</v>
       </c>
@@ -46803,11 +46803,11 @@
       </c>
     </row>
     <row r="20" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
       <c r="F20" s="44" t="s">
         <v>225</v>
       </c>
@@ -47024,11 +47024,11 @@
       <c r="C22" s="17">
         <v>2</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
       <c r="J22" s="14" t="s">
         <v>241</v>
       </c>
@@ -47563,11 +47563,11 @@
       </c>
     </row>
     <row r="27" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
       <c r="F27" t="s">
         <v>100</v>
       </c>
@@ -48001,11 +48001,11 @@
       <c r="C31" s="17">
         <v>0.75</v>
       </c>
-      <c r="F31" s="57" t="s">
+      <c r="F31" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
       <c r="J31" s="6" t="s">
         <v>58</v>
       </c>
@@ -48278,11 +48278,11 @@
       </c>
     </row>
     <row r="34" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
       <c r="J34" s="6" t="s">
         <v>60</v>
       </c>
@@ -48586,11 +48586,11 @@
       </c>
     </row>
     <row r="39" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B39" s="54" t="s">
+      <c r="B39" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
       <c r="J39" s="10" t="s">
         <v>62</v>
       </c>
@@ -48690,11 +48690,11 @@
         <f>IF(C40="wheeled",0.0325,0.014)</f>
         <v>3.2500000000000001E-2</v>
       </c>
-      <c r="J41" s="54" t="s">
+      <c r="J41" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="K41" s="54"/>
-      <c r="L41" s="54"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
       <c r="AF41" s="2">
         <v>37</v>
       </c>
@@ -48892,11 +48892,11 @@
       </c>
     </row>
     <row r="45" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B45" s="54" t="s">
+      <c r="B45" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
       <c r="J45" s="20" t="s">
         <v>72</v>
       </c>
@@ -48939,11 +48939,11 @@
       </c>
     </row>
     <row r="48" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="54"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
@@ -48978,11 +48978,11 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="6" t="s">
@@ -49028,11 +49028,11 @@
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="57" t="s">
+      <c r="B59" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
@@ -49062,11 +49062,11 @@
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="C64" s="55"/>
-      <c r="D64" s="55"/>
+      <c r="C64" s="60"/>
+      <c r="D64" s="60"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="6" t="s">
@@ -49113,11 +49113,11 @@
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55"/>
+      <c r="C70" s="60"/>
+      <c r="D70" s="60"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="6" t="s">
@@ -49164,11 +49164,11 @@
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="54" t="s">
+      <c r="B76" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="54"/>
-      <c r="D76" s="54"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="58"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="6" t="s">
@@ -49215,12 +49215,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B39:D39"/>
@@ -49228,16 +49232,12 @@
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="F31:H31"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B70:D70"/>
   </mergeCells>
   <conditionalFormatting sqref="K31">
     <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="FALSE">
@@ -49315,11 +49315,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="2:45" x14ac:dyDescent="0.2">
       <c r="Y2" s="16" t="s">
@@ -49330,31 +49330,31 @@
       </c>
     </row>
     <row r="3" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="F3" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="N3" s="58" t="s">
         <v>279</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="R3" s="54" t="s">
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="R3" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
       <c r="Y3" s="7" t="s">
         <v>44</v>
       </c>
@@ -50016,11 +50016,11 @@
       <c r="H9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
       <c r="N9" s="6" t="s">
         <v>122</v>
       </c>
@@ -50803,16 +50803,16 @@
       </c>
     </row>
     <row r="16" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="F16" s="57" t="s">
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="F16" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
       <c r="J16" s="12" t="s">
         <v>135</v>
       </c>
@@ -51049,16 +51049,16 @@
       <c r="L18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N18" s="57" t="s">
+      <c r="N18" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="R18" s="57" t="s">
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="R18" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
       <c r="Y18" s="2">
         <v>14</v>
       </c>
@@ -51376,11 +51376,11 @@
       </c>
     </row>
     <row r="21" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
       <c r="F21" s="9" t="s">
         <v>100</v>
       </c>
@@ -51967,11 +51967,11 @@
       <c r="D26" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
       <c r="J26" s="15" t="s">
         <v>67</v>
       </c>
@@ -52190,11 +52190,11 @@
       </c>
     </row>
     <row r="28" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
       <c r="F28" s="6" t="s">
         <v>94</v>
       </c>
@@ -52920,16 +52920,16 @@
       </c>
     </row>
     <row r="35" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="F35" s="57" t="s">
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="F35" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
       <c r="J35" s="11" t="s">
         <v>55</v>
       </c>
@@ -53323,11 +53323,11 @@
       </c>
     </row>
     <row r="40" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
       <c r="Y40" s="2">
         <v>2</v>
       </c>
@@ -53411,11 +53411,11 @@
       <c r="C41" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="J41" s="54" t="s">
+      <c r="J41" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="K41" s="54"/>
-      <c r="L41" s="54"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
       <c r="Y41" s="2">
         <v>3</v>
       </c>
@@ -53827,11 +53827,11 @@
       </c>
     </row>
     <row r="46" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
       <c r="J46" s="15" t="s">
         <v>73</v>
       </c>
@@ -53981,11 +53981,11 @@
       </c>
     </row>
     <row r="49" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
       <c r="Y49" s="2">
         <v>11</v>
       </c>
@@ -54217,11 +54217,11 @@
       </c>
     </row>
     <row r="54" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B54" s="54" t="s">
+      <c r="B54" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
       <c r="Y54" s="2">
         <v>16</v>
       </c>
@@ -54503,11 +54503,11 @@
       </c>
     </row>
     <row r="60" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B60" s="57" t="s">
+      <c r="B60" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
       <c r="Y60" s="2">
         <v>22</v>
       </c>
@@ -54734,11 +54734,11 @@
       </c>
     </row>
     <row r="65" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B65" s="54" t="s">
+      <c r="B65" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
       <c r="Y65" s="2">
         <v>27</v>
       </c>
@@ -54941,11 +54941,11 @@
       </c>
     </row>
     <row r="71" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B71" s="54" t="s">
+      <c r="B71" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="C71" s="55"/>
-      <c r="D71" s="55"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="60"/>
     </row>
     <row r="72" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B72" s="6" t="s">
@@ -54992,11 +54992,11 @@
       </c>
     </row>
     <row r="77" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B77" s="54" t="s">
+      <c r="B77" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="54"/>
-      <c r="D77" s="54"/>
+      <c r="C77" s="58"/>
+      <c r="D77" s="58"/>
     </row>
     <row r="78" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B78" s="6" t="s">
@@ -55043,16 +55043,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="J9:L9"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B65:D65"/>
     <mergeCell ref="B71:D71"/>
@@ -55068,6 +55058,16 @@
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="F35:H35"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="J9:L9"/>
   </mergeCells>
   <conditionalFormatting sqref="K31">
     <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="FALSE">
@@ -55098,8 +55098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8895AA02-1E62-EB44-9405-A51AF8F8C1C2}">
   <dimension ref="B1:CI136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55158,11 +55158,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="2:87" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -55225,26 +55225,26 @@
       <c r="CI2" s="61"/>
     </row>
     <row r="3" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="F3" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="N3" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
       <c r="U3" s="7" t="s">
         <v>44</v>
       </c>
@@ -55325,27 +55325,27 @@
       <c r="AW3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AY3" s="63" t="s">
+      <c r="AY3" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="AZ3" s="63"/>
-      <c r="BA3" s="63"/>
-      <c r="BC3" s="63" t="s">
+      <c r="AZ3" s="62"/>
+      <c r="BA3" s="62"/>
+      <c r="BC3" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="BD3" s="63"/>
-      <c r="BE3" s="63"/>
-      <c r="BG3" s="63" t="s">
+      <c r="BD3" s="62"/>
+      <c r="BE3" s="62"/>
+      <c r="BG3" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="BH3" s="63"/>
-      <c r="BI3" s="63"/>
+      <c r="BH3" s="62"/>
+      <c r="BI3" s="62"/>
       <c r="BJ3" s="2"/>
-      <c r="BK3" s="63" t="s">
+      <c r="BK3" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="BL3" s="63"/>
-      <c r="BM3" s="63"/>
+      <c r="BL3" s="62"/>
+      <c r="BM3" s="62"/>
       <c r="BO3" s="7" t="s">
         <v>44</v>
       </c>
@@ -56570,11 +56570,11 @@
       <c r="H9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
       <c r="N9" s="6" t="s">
         <v>122</v>
       </c>
@@ -57140,7 +57140,7 @@
         <f t="shared" si="20"/>
         <v>70.3125</v>
       </c>
-      <c r="AQ11" s="67" t="s">
+      <c r="AQ11" s="64" t="s">
         <v>181</v>
       </c>
       <c r="AR11" s="3" t="s">
@@ -57348,7 +57348,7 @@
         <f t="shared" si="20"/>
         <v>35.15625</v>
       </c>
-      <c r="AQ12" s="67"/>
+      <c r="AQ12" s="64"/>
       <c r="AR12" s="3" t="s">
         <v>219</v>
       </c>
@@ -57363,16 +57363,16 @@
       <c r="AW12" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="AY12" s="63" t="s">
+      <c r="AY12" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="AZ12" s="63"/>
-      <c r="BA12" s="63"/>
-      <c r="BC12" s="63" t="s">
+      <c r="AZ12" s="62"/>
+      <c r="BA12" s="62"/>
+      <c r="BC12" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="BD12" s="63"/>
-      <c r="BE12" s="63"/>
+      <c r="BD12" s="62"/>
+      <c r="BE12" s="62"/>
       <c r="BG12" s="2" t="s">
         <v>187</v>
       </c>
@@ -57570,7 +57570,7 @@
         <f t="shared" si="20"/>
         <v>17.578125</v>
       </c>
-      <c r="AQ13" s="67"/>
+      <c r="AQ13" s="64"/>
       <c r="AR13" s="3" t="s">
         <v>219</v>
       </c>
@@ -57787,7 +57787,7 @@
         <f t="shared" si="20"/>
         <v>8.7890625</v>
       </c>
-      <c r="AQ14" s="67"/>
+      <c r="AQ14" s="64"/>
       <c r="AR14" s="3" t="s">
         <v>219</v>
       </c>
@@ -57908,11 +57908,11 @@
       </c>
     </row>
     <row r="15" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
       <c r="J15" s="11" t="s">
         <v>55</v>
       </c>
@@ -58005,7 +58005,7 @@
         <f t="shared" si="20"/>
         <v>4.39453125</v>
       </c>
-      <c r="AQ15" s="67"/>
+      <c r="AQ15" s="64"/>
       <c r="AR15" s="3" t="s">
         <v>219</v>
       </c>
@@ -58131,11 +58131,11 @@
       </c>
     </row>
     <row r="16" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
       <c r="F16" s="9" t="s">
         <v>92</v>
       </c>
@@ -58238,7 +58238,7 @@
         <f t="shared" si="20"/>
         <v>2.197265625</v>
       </c>
-      <c r="AQ16" s="67"/>
+      <c r="AQ16" s="64"/>
       <c r="AR16" s="3" t="s">
         <v>219</v>
       </c>
@@ -58466,7 +58466,7 @@
         <f t="shared" si="20"/>
         <v>1.0986328125</v>
       </c>
-      <c r="AQ17" s="67"/>
+      <c r="AQ17" s="64"/>
       <c r="AR17" s="3" t="s">
         <v>219</v>
       </c>
@@ -58615,11 +58615,11 @@
       <c r="L18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N18" s="57" t="s">
+      <c r="N18" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
       <c r="U18" s="2">
         <v>14</v>
       </c>
@@ -58695,7 +58695,7 @@
         <f t="shared" si="20"/>
         <v>0.54931640625</v>
       </c>
-      <c r="AQ18" s="67"/>
+      <c r="AQ18" s="64"/>
       <c r="AR18" s="3" t="s">
         <v>219</v>
       </c>
@@ -58929,7 +58929,7 @@
         <f t="shared" si="20"/>
         <v>0.274658203125</v>
       </c>
-      <c r="AQ19" s="67" t="s">
+      <c r="AQ19" s="64" t="s">
         <v>195</v>
       </c>
       <c r="AR19" s="3">
@@ -59163,7 +59163,7 @@
         <f t="shared" si="20"/>
         <v>0.1373291015625</v>
       </c>
-      <c r="AQ20" s="67"/>
+      <c r="AQ20" s="64"/>
       <c r="AR20" s="3">
         <f>0.358125*($AR$9/2)</f>
         <v>0.54578250000000006</v>
@@ -59270,11 +59270,11 @@
       </c>
     </row>
     <row r="21" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
       <c r="J21" s="14" t="s">
         <v>64</v>
       </c>
@@ -59370,7 +59370,7 @@
         <f t="shared" si="20"/>
         <v>6.866455078125E-2</v>
       </c>
-      <c r="AQ21" s="67"/>
+      <c r="AQ21" s="64"/>
       <c r="AR21" s="3">
         <f>0.456875*($AR$9/2)</f>
         <v>0.69627749999999999</v>
@@ -59379,16 +59379,16 @@
         <v>8</v>
       </c>
       <c r="AW21" s="26"/>
-      <c r="AY21" s="63" t="s">
+      <c r="AY21" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="AZ21" s="63"/>
-      <c r="BA21" s="63"/>
-      <c r="BC21" s="63" t="s">
+      <c r="AZ21" s="62"/>
+      <c r="BA21" s="62"/>
+      <c r="BC21" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="BD21" s="63"/>
-      <c r="BE21" s="63"/>
+      <c r="BD21" s="62"/>
+      <c r="BE21" s="62"/>
       <c r="BG21" s="2"/>
       <c r="BH21" s="2"/>
       <c r="BI21" s="2"/>
@@ -59476,11 +59476,11 @@
       <c r="C22" s="17">
         <v>8</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
       <c r="J22" s="14" t="s">
         <v>241</v>
       </c>
@@ -59573,7 +59573,7 @@
         <f t="shared" si="20"/>
         <v>3.4332275390625E-2</v>
       </c>
-      <c r="AQ22" s="67"/>
+      <c r="AQ22" s="64"/>
       <c r="AR22" s="3">
         <f>0.555625*($AR$9/2)</f>
         <v>0.84677250000000004</v>
@@ -59606,17 +59606,17 @@
       <c r="BE22" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="BG22" s="63" t="s">
+      <c r="BG22" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="BH22" s="63"/>
-      <c r="BI22" s="63"/>
+      <c r="BH22" s="62"/>
+      <c r="BI22" s="62"/>
       <c r="BJ22" s="2"/>
-      <c r="BK22" s="63" t="s">
+      <c r="BK22" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="BL22" s="63"/>
-      <c r="BM22" s="63"/>
+      <c r="BL22" s="62"/>
+      <c r="BM22" s="62"/>
       <c r="BO22" s="2">
         <v>18</v>
       </c>
@@ -59799,7 +59799,7 @@
         <f t="shared" si="20"/>
         <v>1.71661376953125E-2</v>
       </c>
-      <c r="AQ23" s="67"/>
+      <c r="AQ23" s="64"/>
       <c r="AR23" s="3">
         <f>0.654375*($AR$9/2)</f>
         <v>0.99726750000000008</v>
@@ -59807,14 +59807,14 @@
       <c r="AS23" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AU23" s="70" t="s">
+      <c r="AU23" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="AV23" s="67">
+      <c r="AV23" s="64">
         <f>BH20</f>
         <v>8.035629328606575E-9</v>
       </c>
-      <c r="AW23" s="67"/>
+      <c r="AW23" s="64"/>
       <c r="AY23" s="2" t="s">
         <v>158</v>
       </c>
@@ -60038,7 +60038,7 @@
         <f t="shared" si="20"/>
         <v>8.58306884765625E-3</v>
       </c>
-      <c r="AQ24" s="67"/>
+      <c r="AQ24" s="64"/>
       <c r="AR24" s="3">
         <f>0.753125*($AR$9/2)</f>
         <v>1.1477625</v>
@@ -60046,12 +60046,12 @@
       <c r="AS24" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AU24" s="70"/>
-      <c r="AV24" s="67">
+      <c r="AU24" s="63"/>
+      <c r="AV24" s="64">
         <f>BL20</f>
         <v>5.9086911474715009E-9</v>
       </c>
-      <c r="AW24" s="67"/>
+      <c r="AW24" s="64"/>
       <c r="AY24" s="2" t="s">
         <v>163</v>
       </c>
@@ -60278,7 +60278,7 @@
         <f t="shared" si="20"/>
         <v>4.291534423828125E-3</v>
       </c>
-      <c r="AQ25" s="67"/>
+      <c r="AQ25" s="64"/>
       <c r="AR25" s="3">
         <f>0.851875*($AR$9/2)</f>
         <v>1.2982575000000001</v>
@@ -60286,12 +60286,12 @@
       <c r="AS25" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AU25" s="70"/>
-      <c r="AV25" s="67">
+      <c r="AU25" s="63"/>
+      <c r="AV25" s="64">
         <f>BH39</f>
         <v>3.7158728524722129E-9</v>
       </c>
-      <c r="AW25" s="67"/>
+      <c r="AW25" s="64"/>
       <c r="AY25" s="2" t="s">
         <v>167</v>
       </c>
@@ -60518,7 +60518,7 @@
         <f t="shared" si="20"/>
         <v>2.1457672119140625E-3</v>
       </c>
-      <c r="AQ26" s="67"/>
+      <c r="AQ26" s="64"/>
       <c r="AR26" s="3">
         <f>0.950625*($AR$9/2)</f>
         <v>1.4487525000000001</v>
@@ -60526,12 +60526,12 @@
       <c r="AS26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AU26" s="70"/>
-      <c r="AV26" s="67">
+      <c r="AU26" s="63"/>
+      <c r="AV26" s="64">
         <f>BL39</f>
         <v>1.3610837526489838E-9</v>
       </c>
-      <c r="AW26" s="67"/>
+      <c r="AW26" s="64"/>
       <c r="AY26" s="2" t="s">
         <v>170</v>
       </c>
@@ -60748,7 +60748,7 @@
         <f t="shared" si="20"/>
         <v>1.0728836059570312E-3</v>
       </c>
-      <c r="AQ27" s="67" t="s">
+      <c r="AQ27" s="64" t="s">
         <v>204</v>
       </c>
       <c r="AR27" s="3">
@@ -60758,12 +60758,12 @@
       <c r="AS27" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AU27" s="70"/>
-      <c r="AV27" s="67">
+      <c r="AU27" s="63"/>
+      <c r="AV27" s="64">
         <f>BH58</f>
         <v>-5.6457712810376037E-9</v>
       </c>
-      <c r="AW27" s="67"/>
+      <c r="AW27" s="64"/>
       <c r="AY27" s="2" t="s">
         <v>174</v>
       </c>
@@ -60875,11 +60875,11 @@
       </c>
     </row>
     <row r="28" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
       <c r="J28" s="15" t="s">
         <v>69</v>
       </c>
@@ -60972,7 +60972,7 @@
         <f t="shared" si="20"/>
         <v>5.3644180297851562E-4</v>
       </c>
-      <c r="AQ28" s="67"/>
+      <c r="AQ28" s="64"/>
       <c r="AR28" s="3">
         <f>0.530863*($AR$9/2)</f>
         <v>0.80903521199999995</v>
@@ -60980,12 +60980,12 @@
       <c r="AS28" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AU28" s="70"/>
-      <c r="AV28" s="67">
+      <c r="AU28" s="63"/>
+      <c r="AV28" s="64">
         <f>BL58</f>
         <v>-3.968280197497176E-9</v>
       </c>
-      <c r="AW28" s="67"/>
+      <c r="AW28" s="64"/>
       <c r="AY28" s="2" t="s">
         <v>178</v>
       </c>
@@ -61103,11 +61103,11 @@
       <c r="C29" s="17">
         <v>1</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="F29" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
       <c r="J29" s="15" t="s">
         <v>70</v>
       </c>
@@ -61199,7 +61199,7 @@
         <f t="shared" si="20"/>
         <v>2.6822090148925781E-4</v>
       </c>
-      <c r="AQ29" s="67"/>
+      <c r="AQ29" s="64"/>
       <c r="AR29" s="3">
         <f>0.513438*($AR$9/2)</f>
         <v>0.78247951199999999</v>
@@ -61207,12 +61207,12 @@
       <c r="AS29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AU29" s="70"/>
-      <c r="AV29" s="67">
+      <c r="AU29" s="63"/>
+      <c r="AV29" s="64">
         <f>BH77</f>
         <v>-1.4129099626392083E-10</v>
       </c>
-      <c r="AW29" s="67"/>
+      <c r="AW29" s="64"/>
       <c r="BG29" s="2" t="s">
         <v>180</v>
       </c>
@@ -61412,7 +61412,7 @@
         <f t="shared" si="20"/>
         <v>1.3411045074462891E-4</v>
       </c>
-      <c r="AQ30" s="67"/>
+      <c r="AQ30" s="64"/>
       <c r="AR30" s="3">
         <f>0.496013*($AR$9/2)</f>
         <v>0.75592381200000003</v>
@@ -61423,21 +61423,21 @@
       <c r="AU30" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="AV30" s="67" t="b">
+      <c r="AV30" s="64" t="b">
         <f>IF(AV23&lt;0.00001,IF(AV24&lt;0.00001,IF(AV25&lt;0.00001,IF(AV26&lt;0.00001,IF(AV27&lt;0.00001,IF(AV28&lt;0.00001,IF(AV29&lt;0.00001,TRUE,FALSE),FALSE),FALSE),FALSE),FALSE),FALSE),FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AW30" s="67"/>
-      <c r="AY30" s="63" t="s">
+      <c r="AW30" s="64"/>
+      <c r="AY30" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="AZ30" s="63"/>
-      <c r="BA30" s="63"/>
-      <c r="BC30" s="63" t="s">
+      <c r="AZ30" s="62"/>
+      <c r="BA30" s="62"/>
+      <c r="BC30" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="BD30" s="63"/>
-      <c r="BE30" s="63"/>
+      <c r="BD30" s="62"/>
+      <c r="BE30" s="62"/>
       <c r="BG30" s="2" t="s">
         <v>183</v>
       </c>
@@ -61628,7 +61628,7 @@
         <f t="shared" si="20"/>
         <v>6.7055225372314453E-5</v>
       </c>
-      <c r="AQ31" s="67"/>
+      <c r="AQ31" s="64"/>
       <c r="AR31" s="3">
         <f>0.478588*($AR$9/2)</f>
         <v>0.72936811200000007</v>
@@ -61828,7 +61828,7 @@
         <f t="shared" si="20"/>
         <v>3.3527612686157227E-5</v>
       </c>
-      <c r="AQ32" s="67"/>
+      <c r="AQ32" s="64"/>
       <c r="AR32" s="3">
         <f>0.461163*($AR$9/2)</f>
         <v>0.702812412</v>
@@ -62036,7 +62036,7 @@
         <f t="shared" si="20"/>
         <v>1.6763806343078613E-5</v>
       </c>
-      <c r="AQ33" s="67"/>
+      <c r="AQ33" s="64"/>
       <c r="AR33" s="3">
         <f>0.443738*($AR$9/2)</f>
         <v>0.67625671200000004</v>
@@ -62239,7 +62239,7 @@
         <f t="shared" si="20"/>
         <v>8.3819031715393066E-6</v>
       </c>
-      <c r="AQ34" s="67"/>
+      <c r="AQ34" s="64"/>
       <c r="AR34" s="3">
         <f>0.426313*($AR$9/2)</f>
         <v>0.64970101199999997</v>
@@ -62357,11 +62357,11 @@
       </c>
     </row>
     <row r="35" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
       <c r="J35" s="11" t="s">
         <v>55</v>
       </c>
@@ -62408,7 +62408,7 @@
         <f t="shared" si="20"/>
         <v>4.1909515857696533E-6</v>
       </c>
-      <c r="AQ35" s="67" t="s">
+      <c r="AQ35" s="64" t="s">
         <v>223</v>
       </c>
       <c r="AR35" s="3">
@@ -62513,7 +62513,7 @@
         <f t="shared" si="20"/>
         <v>2.0954757928848267E-6</v>
       </c>
-      <c r="AQ36" s="67"/>
+      <c r="AQ36" s="64"/>
       <c r="AR36" s="3">
         <v>5.8781249999999998</v>
       </c>
@@ -62637,7 +62637,7 @@
         <f t="shared" si="20"/>
         <v>1.0477378964424133E-6</v>
       </c>
-      <c r="AQ37" s="67"/>
+      <c r="AQ37" s="64"/>
       <c r="AR37" s="3">
         <v>4.3968749999999996</v>
       </c>
@@ -62797,7 +62797,7 @@
         <f t="shared" si="20"/>
         <v>5.2386894822120667E-7</v>
       </c>
-      <c r="AQ38" s="67"/>
+      <c r="AQ38" s="64"/>
       <c r="AR38" s="3">
         <v>2.9156249999999999</v>
       </c>
@@ -62910,7 +62910,7 @@
         <f t="shared" si="20"/>
         <v>2.6193447411060333E-7</v>
       </c>
-      <c r="AQ39" s="67"/>
+      <c r="AQ39" s="64"/>
       <c r="AR39" s="3">
         <v>1.434375</v>
       </c>
@@ -63013,11 +63013,11 @@
       </c>
     </row>
     <row r="40" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
       <c r="AF40" s="2">
         <v>36</v>
       </c>
@@ -63054,7 +63054,7 @@
         <f t="shared" si="20"/>
         <v>1.3096723705530167E-7</v>
       </c>
-      <c r="AQ40" s="67"/>
+      <c r="AQ40" s="64"/>
       <c r="AR40" s="3">
         <v>-4.6875E-2</v>
       </c>
@@ -63141,11 +63141,11 @@
       <c r="C41" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="J41" s="54" t="s">
+      <c r="J41" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="K41" s="54"/>
-      <c r="L41" s="54"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
       <c r="AF41" s="2">
         <v>37</v>
       </c>
@@ -63182,7 +63182,7 @@
         <f t="shared" si="20"/>
         <v>6.5483618527650833E-8</v>
       </c>
-      <c r="AQ41" s="67"/>
+      <c r="AQ41" s="64"/>
       <c r="AR41" s="3">
         <v>-1.528125</v>
       </c>
@@ -63192,10 +63192,10 @@
       <c r="AU41" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="AV41" s="69" t="s">
+      <c r="AV41" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="AW41" s="69"/>
+      <c r="AW41" s="66"/>
       <c r="AX41" s="24"/>
       <c r="AY41" s="24"/>
       <c r="AZ41" s="24"/>
@@ -63204,17 +63204,17 @@
       <c r="BC41" s="24"/>
       <c r="BD41" s="24"/>
       <c r="BE41" s="25"/>
-      <c r="BG41" s="63" t="s">
+      <c r="BG41" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="BH41" s="63"/>
-      <c r="BI41" s="63"/>
+      <c r="BH41" s="62"/>
+      <c r="BI41" s="62"/>
       <c r="BJ41" s="2"/>
-      <c r="BK41" s="63" t="s">
+      <c r="BK41" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="BL41" s="63"/>
-      <c r="BM41" s="63"/>
+      <c r="BL41" s="62"/>
+      <c r="BM41" s="62"/>
       <c r="BO41" s="2">
         <v>3</v>
       </c>
@@ -63342,7 +63342,7 @@
         <f t="shared" si="20"/>
         <v>3.2741809263825417E-8</v>
       </c>
-      <c r="AQ42" s="67"/>
+      <c r="AQ42" s="64"/>
       <c r="AR42" s="3">
         <v>-3.0093749999999999</v>
       </c>
@@ -63350,22 +63350,22 @@
         <v>43</v>
       </c>
       <c r="AU42" s="27"/>
-      <c r="AV42" s="70" t="s">
+      <c r="AV42" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="AW42" s="70"/>
-      <c r="AX42" s="70"/>
-      <c r="AY42" s="70" t="s">
+      <c r="AW42" s="63"/>
+      <c r="AX42" s="63"/>
+      <c r="AY42" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="AZ42" s="70"/>
-      <c r="BA42" s="70"/>
-      <c r="BB42" s="70"/>
-      <c r="BC42" s="70" t="s">
+      <c r="AZ42" s="63"/>
+      <c r="BA42" s="63"/>
+      <c r="BB42" s="63"/>
+      <c r="BC42" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="BD42" s="70"/>
-      <c r="BE42" s="71"/>
+      <c r="BD42" s="63"/>
+      <c r="BE42" s="65"/>
       <c r="BG42" s="28" t="s">
         <v>154</v>
       </c>
@@ -63529,10 +63529,10 @@
       <c r="AX43" s="2">
         <v>-9.5</v>
       </c>
-      <c r="AY43" s="70" t="s">
+      <c r="AY43" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="AZ43" s="70"/>
+      <c r="AZ43" s="63"/>
       <c r="BA43" s="2">
         <v>-9.5</v>
       </c>
@@ -63976,11 +63976,11 @@
       </c>
     </row>
     <row r="46" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
       <c r="J46" s="15" t="s">
         <v>73</v>
       </c>
@@ -64108,19 +64108,19 @@
       <c r="L47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AF47" s="70" t="s">
+      <c r="AF47" s="63" t="s">
         <v>222</v>
       </c>
-      <c r="AG47" s="70"/>
-      <c r="AH47" s="70"/>
-      <c r="AI47" s="70"/>
+      <c r="AG47" s="63"/>
+      <c r="AH47" s="63"/>
+      <c r="AI47" s="63"/>
       <c r="AU47" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="AV47" s="69" t="s">
+      <c r="AV47" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="AW47" s="69"/>
+      <c r="AW47" s="66"/>
       <c r="AX47" s="24"/>
       <c r="AY47" s="24"/>
       <c r="AZ47" s="24"/>
@@ -64250,21 +64250,21 @@
         <v>53</v>
       </c>
       <c r="AU48" s="27"/>
-      <c r="AV48" s="70" t="s">
+      <c r="AV48" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="AW48" s="70"/>
-      <c r="AX48" s="70"/>
-      <c r="AY48" s="70" t="s">
+      <c r="AW48" s="63"/>
+      <c r="AX48" s="63"/>
+      <c r="AY48" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="AZ48" s="70"/>
-      <c r="BA48" s="70"/>
-      <c r="BB48" s="70" t="s">
+      <c r="AZ48" s="63"/>
+      <c r="BA48" s="63"/>
+      <c r="BB48" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="BC48" s="70"/>
-      <c r="BD48" s="71"/>
+      <c r="BC48" s="63"/>
+      <c r="BD48" s="65"/>
       <c r="BG48" s="2" t="s">
         <v>180</v>
       </c>
@@ -64356,11 +64356,11 @@
       </c>
     </row>
     <row r="49" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
       <c r="AF49" s="2">
         <v>0</v>
       </c>
@@ -64538,7 +64538,7 @@
         <f t="shared" ref="AO50:AO79" si="42">AI50-AG50</f>
         <v>1450</v>
       </c>
-      <c r="AU50" s="72" t="s">
+      <c r="AU50" s="70" t="s">
         <v>160</v>
       </c>
       <c r="AV50" s="51">
@@ -64705,7 +64705,7 @@
         <f t="shared" si="42"/>
         <v>725</v>
       </c>
-      <c r="AU51" s="72"/>
+      <c r="AU51" s="70"/>
       <c r="AV51" s="27">
         <v>-1.1499587328259999E-4</v>
       </c>
@@ -64870,22 +64870,22 @@
         <f t="shared" si="42"/>
         <v>362.5</v>
       </c>
-      <c r="AU52" s="72"/>
-      <c r="AV52" s="64">
+      <c r="AU52" s="70"/>
+      <c r="AV52" s="67">
         <v>-2.4012358386552801</v>
       </c>
-      <c r="AW52" s="65"/>
-      <c r="AX52" s="66"/>
-      <c r="AY52" s="64">
+      <c r="AW52" s="68"/>
+      <c r="AX52" s="69"/>
+      <c r="AY52" s="67">
         <v>0.149391545914075</v>
       </c>
-      <c r="AZ52" s="65"/>
-      <c r="BA52" s="66"/>
-      <c r="BB52" s="64">
+      <c r="AZ52" s="68"/>
+      <c r="BA52" s="69"/>
+      <c r="BB52" s="67">
         <v>3.65120250353774</v>
       </c>
-      <c r="BC52" s="65"/>
-      <c r="BD52" s="66"/>
+      <c r="BC52" s="68"/>
+      <c r="BD52" s="69"/>
       <c r="BG52" s="2" t="s">
         <v>190</v>
       </c>
@@ -65013,7 +65013,7 @@
         <f t="shared" si="42"/>
         <v>181.25</v>
       </c>
-      <c r="AU53" s="72" t="s">
+      <c r="AU53" s="70" t="s">
         <v>164</v>
       </c>
       <c r="AV53" s="51">
@@ -65134,11 +65134,11 @@
       </c>
     </row>
     <row r="54" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B54" s="54" t="s">
+      <c r="B54" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
       <c r="AF54" s="2">
         <v>5</v>
       </c>
@@ -65175,7 +65175,7 @@
         <f t="shared" si="42"/>
         <v>90.625</v>
       </c>
-      <c r="AU54" s="72"/>
+      <c r="AU54" s="70"/>
       <c r="AV54" s="27">
         <v>-2.5152080542999999E-6</v>
       </c>
@@ -65336,22 +65336,22 @@
         <f t="shared" si="42"/>
         <v>45.3125</v>
       </c>
-      <c r="AU55" s="73"/>
-      <c r="AV55" s="64">
+      <c r="AU55" s="71"/>
+      <c r="AV55" s="67">
         <v>-1.5880058514071E-2</v>
       </c>
-      <c r="AW55" s="65"/>
-      <c r="AX55" s="66"/>
-      <c r="AY55" s="65">
+      <c r="AW55" s="68"/>
+      <c r="AX55" s="69"/>
+      <c r="AY55" s="68">
         <v>0.110802661807325</v>
       </c>
-      <c r="AZ55" s="65"/>
-      <c r="BA55" s="65"/>
-      <c r="BB55" s="64">
+      <c r="AZ55" s="68"/>
+      <c r="BA55" s="68"/>
+      <c r="BB55" s="67">
         <v>7.4721088420790002E-3</v>
       </c>
-      <c r="BC55" s="65"/>
-      <c r="BD55" s="66"/>
+      <c r="BC55" s="68"/>
+      <c r="BD55" s="69"/>
       <c r="BG55" s="2" t="s">
         <v>194</v>
       </c>
@@ -65970,11 +65970,11 @@
       </c>
     </row>
     <row r="60" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B60" s="57" t="s">
+      <c r="B60" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
       <c r="AF60" s="2">
         <v>11</v>
       </c>
@@ -66011,17 +66011,17 @@
         <f t="shared" si="42"/>
         <v>1.416015625</v>
       </c>
-      <c r="BG60" s="63" t="s">
+      <c r="BG60" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="BH60" s="63"/>
-      <c r="BI60" s="63"/>
+      <c r="BH60" s="62"/>
+      <c r="BI60" s="62"/>
       <c r="BJ60" s="2"/>
-      <c r="BK60" s="63" t="s">
+      <c r="BK60" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="BL60" s="63"/>
-      <c r="BM60" s="63"/>
+      <c r="BL60" s="62"/>
+      <c r="BM60" s="62"/>
       <c r="BO60" s="2">
         <v>22</v>
       </c>
@@ -66641,11 +66641,11 @@
       </c>
     </row>
     <row r="65" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B65" s="54" t="s">
+      <c r="B65" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
       <c r="AF65" s="2">
         <v>16</v>
       </c>
@@ -67327,11 +67327,11 @@
       <c r="CI70" s="61"/>
     </row>
     <row r="71" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B71" s="54" t="s">
+      <c r="B71" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="C71" s="55"/>
-      <c r="D71" s="55"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="60"/>
       <c r="AF71" s="2">
         <v>22</v>
       </c>
@@ -67639,7 +67639,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="BU73" s="2">
-        <f t="dataTable" ref="BU73:BU102" dt2D="0" dtr="0" r1="BH42" ca="1"/>
+        <f t="dataTable" ref="BU73:BU102" dt2D="0" dtr="0" r1="BH42"/>
         <v>1.1118383357407486</v>
       </c>
       <c r="BV73" s="2">
@@ -67678,7 +67678,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="CF73" s="2">
-        <f t="dataTable" ref="CF73:CF102" dt2D="0" dtr="0" r1="BL42" ca="1"/>
+        <f t="dataTable" ref="CF73:CF102" dt2D="0" dtr="0" r1="BL42"/>
         <v>1.1162112792863177</v>
       </c>
       <c r="CG73" s="2">
@@ -68093,11 +68093,11 @@
       </c>
     </row>
     <row r="77" spans="2:87" x14ac:dyDescent="0.2">
-      <c r="B77" s="54" t="s">
+      <c r="B77" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="54"/>
-      <c r="D77" s="54"/>
+      <c r="C77" s="58"/>
+      <c r="D77" s="58"/>
       <c r="AF77" s="2">
         <v>28</v>
       </c>
@@ -70335,7 +70335,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="BU107" s="2">
-        <f t="dataTable" ref="BU107:BU136" dt2D="0" dtr="0" r1="BH61" ca="1"/>
+        <f t="dataTable" ref="BU107:BU136" dt2D="0" dtr="0" r1="BH61"/>
         <v>1.1358906375579021</v>
       </c>
       <c r="BV107" s="2">
@@ -70374,7 +70374,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="CF107" s="2">
-        <f t="dataTable" ref="CF107:CF136" dt2D="0" dtr="0" r1="BL61" ca="1"/>
+        <f t="dataTable" ref="CF107:CF136" dt2D="0" dtr="0" r1="BL61"/>
         <v>1.2201332261292821</v>
       </c>
       <c r="CG107" s="2">
@@ -72538,17 +72538,66 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="BB52:BD52"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="AY52:BA52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="AV47:AW47"/>
-    <mergeCell ref="AV48:AX48"/>
-    <mergeCell ref="AU50:AU52"/>
-    <mergeCell ref="AV52:AX52"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="AQ7:AS7"/>
+    <mergeCell ref="AQ2:AS2"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="AY2:BE2"/>
+    <mergeCell ref="AU9:AW9"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="BC30:BE30"/>
+    <mergeCell ref="AQ35:AQ42"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="AV42:AX42"/>
+    <mergeCell ref="AY42:BB42"/>
+    <mergeCell ref="BC42:BE42"/>
+    <mergeCell ref="AQ27:AQ34"/>
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="AY30:BA30"/>
+    <mergeCell ref="AQ19:AQ26"/>
+    <mergeCell ref="AY21:BA21"/>
+    <mergeCell ref="BC21:BE21"/>
+    <mergeCell ref="AU53:AU55"/>
+    <mergeCell ref="AV55:AX55"/>
+    <mergeCell ref="AQ11:AQ18"/>
+    <mergeCell ref="AY12:BA12"/>
+    <mergeCell ref="BC12:BE12"/>
+    <mergeCell ref="BK22:BM22"/>
+    <mergeCell ref="AU23:AU29"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="AV24:AW24"/>
+    <mergeCell ref="AV25:AW25"/>
+    <mergeCell ref="AV26:AW26"/>
+    <mergeCell ref="BG22:BI22"/>
+    <mergeCell ref="AV27:AW27"/>
+    <mergeCell ref="AV28:AW28"/>
+    <mergeCell ref="AV29:AW29"/>
+    <mergeCell ref="AU14:AW14"/>
+    <mergeCell ref="AU22:AW22"/>
+    <mergeCell ref="BO36:BX36"/>
+    <mergeCell ref="BZ36:CI36"/>
+    <mergeCell ref="AV41:AW41"/>
+    <mergeCell ref="BG41:BI41"/>
+    <mergeCell ref="BK41:BM41"/>
+    <mergeCell ref="BZ2:CI2"/>
+    <mergeCell ref="AY3:BA3"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BG3:BI3"/>
+    <mergeCell ref="BK3:BM3"/>
+    <mergeCell ref="BG2:BM2"/>
+    <mergeCell ref="BO2:BX2"/>
     <mergeCell ref="BO104:BX104"/>
     <mergeCell ref="BZ104:CI104"/>
     <mergeCell ref="B65:D65"/>
@@ -72565,66 +72614,17 @@
     <mergeCell ref="BB55:BD55"/>
     <mergeCell ref="AY48:BA48"/>
     <mergeCell ref="BB48:BD48"/>
-    <mergeCell ref="BZ2:CI2"/>
-    <mergeCell ref="AY3:BA3"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BG3:BI3"/>
-    <mergeCell ref="BK3:BM3"/>
-    <mergeCell ref="BG2:BM2"/>
-    <mergeCell ref="BO2:BX2"/>
-    <mergeCell ref="BO36:BX36"/>
-    <mergeCell ref="BZ36:CI36"/>
-    <mergeCell ref="AV41:AW41"/>
-    <mergeCell ref="BG41:BI41"/>
-    <mergeCell ref="BK41:BM41"/>
-    <mergeCell ref="AQ11:AQ18"/>
-    <mergeCell ref="AY12:BA12"/>
-    <mergeCell ref="BC12:BE12"/>
-    <mergeCell ref="BK22:BM22"/>
-    <mergeCell ref="AU23:AU29"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="AV24:AW24"/>
-    <mergeCell ref="AV25:AW25"/>
-    <mergeCell ref="AV26:AW26"/>
-    <mergeCell ref="BG22:BI22"/>
-    <mergeCell ref="AV27:AW27"/>
-    <mergeCell ref="AV28:AW28"/>
-    <mergeCell ref="AV29:AW29"/>
-    <mergeCell ref="AU14:AW14"/>
-    <mergeCell ref="AU22:AW22"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="BC30:BE30"/>
-    <mergeCell ref="AQ35:AQ42"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="AV42:AX42"/>
-    <mergeCell ref="AY42:BB42"/>
-    <mergeCell ref="BC42:BE42"/>
-    <mergeCell ref="AQ27:AQ34"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="AY30:BA30"/>
-    <mergeCell ref="AQ19:AQ26"/>
-    <mergeCell ref="AY21:BA21"/>
-    <mergeCell ref="BC21:BE21"/>
-    <mergeCell ref="AU53:AU55"/>
-    <mergeCell ref="AV55:AX55"/>
-    <mergeCell ref="AQ7:AS7"/>
-    <mergeCell ref="AQ2:AS2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="AY2:BE2"/>
-    <mergeCell ref="AU9:AW9"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="AV47:AW47"/>
+    <mergeCell ref="AV48:AX48"/>
+    <mergeCell ref="AU50:AU52"/>
+    <mergeCell ref="AV52:AX52"/>
+    <mergeCell ref="BB52:BD52"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="AY52:BA52"/>
   </mergeCells>
   <conditionalFormatting sqref="G12">
     <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="FALSE">

</xml_diff>